<commit_message>
updated dashboard and products and orders
</commit_message>
<xml_diff>
--- a/retailer/data/products.xlsx
+++ b/retailer/data/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f5092fb7e2292c0/Desktop/retailer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_23F921EDB96B8E3EDF2C4C48D5B0133C494A8294" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBC8AA50-4717-41F4-A85D-B212A91450E7}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_23F921EDB96B8E3EDF2C4C48D5B0133C494A8294" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE4952B9-EC01-4DFB-B47A-DAE944604782}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="116">
   <si>
     <t>product_id</t>
   </si>
@@ -362,13 +362,19 @@
   </si>
   <si>
     <t>Out of Stock</t>
+  </si>
+  <si>
+    <t>supplier_name</t>
+  </si>
+  <si>
+    <t>Global Suppliers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +389,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -420,11 +438,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,6 +460,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -729,9 +753,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -741,9 +767,10 @@
     <col min="4" max="4" width="19.265625" customWidth="1"/>
     <col min="5" max="5" width="14.73046875" customWidth="1"/>
     <col min="6" max="6" width="22.73046875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,8 +789,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -782,8 +812,11 @@
       <c r="F2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -802,8 +835,11 @@
       <c r="F3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -822,8 +858,11 @@
       <c r="F4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -842,8 +881,11 @@
       <c r="F5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G5" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -862,8 +904,11 @@
       <c r="F6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -882,8 +927,11 @@
       <c r="F7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G7" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -902,8 +950,11 @@
       <c r="F8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G8" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -922,8 +973,11 @@
       <c r="F9" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -942,8 +996,11 @@
       <c r="F10" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G10" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -962,8 +1019,11 @@
       <c r="F11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G11" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -982,8 +1042,11 @@
       <c r="F12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G12" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1002,8 +1065,11 @@
       <c r="F13" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G13" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1022,8 +1088,11 @@
       <c r="F14" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G14" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1042,8 +1111,11 @@
       <c r="F15" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G15" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1062,8 +1134,11 @@
       <c r="F16" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1082,8 +1157,11 @@
       <c r="F17" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1102,8 +1180,11 @@
       <c r="F18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1122,8 +1203,11 @@
       <c r="F19" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G19" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1142,8 +1226,11 @@
       <c r="F20" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G20" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1162,8 +1249,11 @@
       <c r="F21" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G21" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1182,8 +1272,11 @@
       <c r="F22" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G22" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1202,8 +1295,11 @@
       <c r="F23" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G23" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1222,8 +1318,11 @@
       <c r="F24" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G24" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1242,8 +1341,11 @@
       <c r="F25" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G25" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1262,8 +1364,11 @@
       <c r="F26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G26" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1282,8 +1387,11 @@
       <c r="F27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G27" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1302,8 +1410,11 @@
       <c r="F28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G28" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1322,8 +1433,11 @@
       <c r="F29" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G29" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1342,8 +1456,11 @@
       <c r="F30" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G30" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1362,8 +1479,11 @@
       <c r="F31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G31" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1382,8 +1502,11 @@
       <c r="F32" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G32" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1402,8 +1525,11 @@
       <c r="F33" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G33" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1422,8 +1548,11 @@
       <c r="F34" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G34" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1442,8 +1571,11 @@
       <c r="F35" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G35" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1462,8 +1594,11 @@
       <c r="F36" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G36" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1482,8 +1617,11 @@
       <c r="F37" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G37" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1502,8 +1640,11 @@
       <c r="F38" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G38" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1522,8 +1663,11 @@
       <c r="F39" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G39" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1542,8 +1686,11 @@
       <c r="F40" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G40" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1562,8 +1709,11 @@
       <c r="F41" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G41" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1582,8 +1732,11 @@
       <c r="F42" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G42" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1602,8 +1755,11 @@
       <c r="F43" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G43" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1622,8 +1778,11 @@
       <c r="F44" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G44" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1642,8 +1801,11 @@
       <c r="F45" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G45" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1662,8 +1824,11 @@
       <c r="F46" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G46" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1682,8 +1847,11 @@
       <c r="F47" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G47" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1702,8 +1870,11 @@
       <c r="F48" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G48" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1722,8 +1893,11 @@
       <c r="F49" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G49" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1742,8 +1916,11 @@
       <c r="F50" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G50" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1761,6 +1938,9 @@
       </c>
       <c r="F51" t="s">
         <v>111</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>